<commit_message>
Add DenseNet brightness_contrast augmentation
</commit_message>
<xml_diff>
--- a/models/basic_CNN/Experiments.xlsx
+++ b/models/basic_CNN/Experiments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micha\Desktop\repozytoria\DeepLearning_WUT\models\basic_CNN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{234050EE-6114-48BD-991C-7F441BC699F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B07B549-8E4E-4345-A03B-895FCB703CCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{E1AFF237-2CE8-439A-961A-F738235F199A}"/>
   </bookViews>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="65">
   <si>
     <t>Augmentations</t>
   </si>
@@ -2794,6 +2794,13 @@
   <si>
     <t>epoch 45 TRAIN error: 1.1047, acc: 0.6120
 epoch 45 VALIDATION error: 0.8677, acc: 0.6915</t>
+  </si>
+  <si>
+    <t>brightness_contrast</t>
+  </si>
+  <si>
+    <t>epoch 48 TRAIN error: 0.7410, acc: 0.7371
+epoch 48 VALIDATION error: 0.7566, acc: 0.7420</t>
   </si>
 </sst>
 </file>
@@ -3778,7 +3785,7 @@
   <dimension ref="B2:S31"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4484,6 +4491,23 @@
         <v>56</v>
       </c>
     </row>
+    <row r="18" spans="2:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="B18" s="4">
+        <v>14</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="O18" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="P18" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.25">
       <c r="P27" t="s">
         <v>33</v>

</xml_diff>